<commit_message>
added photo upload feature
</commit_message>
<xml_diff>
--- a/complaints.xlsx
+++ b/complaints.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,6 +468,16 @@
           <t>Location_Keywords</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Complaint_ID</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Photo_Filename</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
@@ -498,6 +508,8 @@
           <t>in area, There</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
@@ -528,6 +540,8 @@
           <t>in our, The</t>
         </is>
       </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
@@ -558,6 +572,8 @@
           <t>in our, The</t>
         </is>
       </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -588,6 +604,8 @@
           <t>near the, Unauthorized, area is</t>
         </is>
       </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -618,6 +636,8 @@
           <t>near the, The</t>
         </is>
       </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -648,6 +668,8 @@
           <t>at any</t>
         </is>
       </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -678,6 +700,8 @@
           <t>road after, near the, An</t>
         </is>
       </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
@@ -706,6 +730,48 @@
       <c r="F9" t="inlineStr">
         <is>
           <t>in medical</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>45945.78909712595</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>richard</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Streetlights in our neighborhood are flickering at night, making it difficult to walk safely. It needs to be checked soon.</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Roads</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>at night,, Streetlights, in our</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>COMP_20251015_185617_5606</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>complaint_COMP_20251015_185617_5606_20251015_185617_20251015_185617.jpeg</t>
         </is>
       </c>
     </row>

</xml_diff>